<commit_message>
Big Service Updates and Unity Connection Update
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Übersicht über alle Bestellungen</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Dauer</t>
   </si>
   <si>
-    <t>bestellung3834</t>
+    <t>bestellung1411</t>
   </si>
   <si>
     <t>Fahrrad</t>
@@ -56,7 +56,7 @@
     <t>kundePruefen</t>
   </si>
   <si>
-    <t>Justin Torres</t>
+    <t>Travis Garcia</t>
   </si>
   <si>
     <t>bestellungSichten</t>
@@ -74,34 +74,46 @@
     <t>bedarfPruefen</t>
   </si>
   <si>
-    <t>Travis Butler</t>
+    <t>John Brown</t>
   </si>
   <si>
     <t>bedarfNachbearbeiten</t>
   </si>
   <si>
-    <t>problemBeschreiben</t>
-  </si>
-  <si>
     <t>stuecklisteBetrachten</t>
   </si>
   <si>
-    <t>rohmaterialVerfuegbarkeitPruefen</t>
-  </si>
-  <si>
-    <t>materialbedarfErstellen</t>
-  </si>
-  <si>
     <t>produktionsauftragErstellen</t>
   </si>
   <si>
+    <t>produktionsauftragBegutachten</t>
+  </si>
+  <si>
+    <t>Roberto Müller</t>
+  </si>
+  <si>
+    <t>transportieren</t>
+  </si>
+  <si>
+    <t>Förderband 0</t>
+  </si>
+  <si>
+    <t>bearbeiten</t>
+  </si>
+  <si>
+    <t>Maschine 0</t>
+  </si>
+  <si>
+    <t>kommissionieren</t>
+  </si>
+  <si>
+    <t>auftragsbestaetigungErstellen</t>
+  </si>
+  <si>
     <t>rechnungErstellen</t>
   </si>
   <si>
-    <t>Frank Müller</t>
-  </si>
-  <si>
-    <t>auftragsbestaetigungErstellen</t>
+    <t>Justin Gonzalez</t>
   </si>
   <si>
     <t>auftragsbestaetigungSenden</t>
@@ -196,13 +208,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>44841.2501701</v>
+        <v>44886.3230445</v>
       </c>
       <c r="E3" s="1">
-        <v>44841.3411423</v>
+        <v>44886.3688778</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>7860</v>
+        <v>3960</v>
       </c>
     </row>
   </sheetData>
@@ -212,7 +224,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -254,10 +266,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="1">
-        <v>44841.2501701</v>
+        <v>44886.3230445</v>
       </c>
       <c r="E3" s="1">
-        <v>44841.2529479</v>
+        <v>44886.3258222</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>240</v>
@@ -274,13 +286,13 @@
         <v>14</v>
       </c>
       <c r="D4" s="1">
-        <v>44841.2529479</v>
+        <v>44886.3258222</v>
       </c>
       <c r="E4" s="1">
-        <v>44841.2564201</v>
+        <v>44886.3306833</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>300</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -294,13 +306,13 @@
         <v>14</v>
       </c>
       <c r="D5" s="1">
-        <v>44841.2564201</v>
+        <v>44886.3306833</v>
       </c>
       <c r="E5" s="1">
-        <v>44841.2598923</v>
+        <v>44886.3320722</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>300</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -314,10 +326,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="1">
-        <v>44841.2598923</v>
+        <v>44886.3320722</v>
       </c>
       <c r="E6" s="1">
-        <v>44841.2626701</v>
+        <v>44886.33485</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>240</v>
@@ -334,13 +346,13 @@
         <v>14</v>
       </c>
       <c r="D7" s="1">
-        <v>44841.2626701</v>
+        <v>44886.33485</v>
       </c>
       <c r="E7" s="1">
-        <v>44841.276559</v>
+        <v>44886.3355445</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>1200</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -354,10 +366,10 @@
         <v>20</v>
       </c>
       <c r="D8" s="1">
-        <v>44841.276559</v>
+        <v>44886.3355445</v>
       </c>
       <c r="E8" s="1">
-        <v>44841.2800312</v>
+        <v>44886.3390167</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>300</v>
@@ -374,10 +386,10 @@
         <v>20</v>
       </c>
       <c r="D9" s="1">
-        <v>44841.2800312</v>
+        <v>44886.3390167</v>
       </c>
       <c r="E9" s="1">
-        <v>44841.2835034</v>
+        <v>44886.3424889</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>300</v>
@@ -394,10 +406,10 @@
         <v>20</v>
       </c>
       <c r="D10" s="1">
-        <v>44841.2835034</v>
+        <v>44886.3424889</v>
       </c>
       <c r="E10" s="1">
-        <v>44841.2869757</v>
+        <v>44886.3459611</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>300</v>
@@ -408,16 +420,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="1">
-        <v>44841.2869757</v>
+        <v>44886.3459611</v>
       </c>
       <c r="E11" s="1">
-        <v>44841.2904479</v>
+        <v>44886.3494333</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>300</v>
@@ -428,19 +440,19 @@
         <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1">
-        <v>44841.2904479</v>
+        <v>44886.3494333</v>
       </c>
       <c r="E12" s="1">
-        <v>44841.2939201</v>
+        <v>44886.3542945</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>300</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -448,19 +460,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1">
-        <v>44841.2939201</v>
+        <v>44886.3542945</v>
       </c>
       <c r="E13" s="1">
-        <v>44841.2973923</v>
+        <v>44886.3549889</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>300</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -468,19 +480,19 @@
         <v>7</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1">
-        <v>44841.2973923</v>
+        <v>44886.3549889</v>
       </c>
       <c r="E14" s="1">
-        <v>44841.3008646</v>
+        <v>44886.3570722</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>300</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -488,19 +500,19 @@
         <v>7</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1">
-        <v>44841.3008646</v>
+        <v>44886.3570722</v>
       </c>
       <c r="E15" s="1">
-        <v>44841.3043368</v>
+        <v>44886.3584611</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>300</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -508,19 +520,19 @@
         <v>7</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1">
-        <v>44841.3043368</v>
+        <v>44886.3584611</v>
       </c>
       <c r="E16" s="1">
-        <v>44841.307809</v>
+        <v>44886.3654056</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -528,19 +540,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1">
-        <v>44841.307809</v>
+        <v>44886.3612389</v>
       </c>
       <c r="E17" s="1">
-        <v>44841.3085034</v>
+        <v>44886.3681833</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>60</v>
+        <v>600</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -548,178 +560,18 @@
         <v>7</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1">
-        <v>44841.3085034</v>
+        <v>44886.3681833</v>
       </c>
       <c r="E18" s="1">
-        <v>44841.3119757</v>
+        <v>44886.3688778</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1">
-        <v>44841.3119757</v>
-      </c>
-      <c r="E19" s="1">
-        <v>44841.3154479</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="1">
-        <v>44841.3154479</v>
-      </c>
-      <c r="E20" s="1">
-        <v>44841.3161423</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="1">
-        <v>44841.3161423</v>
-      </c>
-      <c r="E21" s="1">
-        <v>44841.3196146</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="1">
-        <v>44841.3196146</v>
-      </c>
-      <c r="E22" s="1">
-        <v>44841.3230868</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="1">
-        <v>44841.3230868</v>
-      </c>
-      <c r="E23" s="1">
-        <v>44841.326559</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="1">
-        <v>44841.326559</v>
-      </c>
-      <c r="E24" s="1">
-        <v>44841.3335034</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="1">
-        <v>44841.3335034</v>
-      </c>
-      <c r="E25" s="1">
-        <v>44841.3404479</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="1">
-        <v>44841.3404479</v>
-      </c>
-      <c r="E26" s="1">
-        <v>44841.3411423</v>
-      </c>
-      <c r="F26" s="0" t="n">
         <v>60</v>
       </c>
     </row>

</xml_diff>